<commit_message>
Removed solutions folder fix gitignore
</commit_message>
<xml_diff>
--- a/CS221/TimeLog.xlsx
+++ b/CS221/TimeLog.xlsx
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Lectures</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>Final result</t>
+  </si>
+  <si>
+    <t>Overall</t>
   </si>
 </sst>
 </file>
@@ -541,11 +544,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="234081664"/>
-        <c:axId val="234609664"/>
+        <c:axId val="199500544"/>
+        <c:axId val="199502080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="234081664"/>
+        <c:axId val="199500544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -554,7 +557,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="234609664"/>
+        <c:crossAx val="199502080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -562,7 +565,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="234609664"/>
+        <c:axId val="199502080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -573,7 +576,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="234081664"/>
+        <c:crossAx val="199500544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -685,11 +688,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137325568"/>
-        <c:axId val="137327360"/>
+        <c:axId val="199530752"/>
+        <c:axId val="199536640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137325568"/>
+        <c:axId val="199530752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -698,7 +701,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137327360"/>
+        <c:crossAx val="199536640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -706,7 +709,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137327360"/>
+        <c:axId val="199536640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -717,7 +720,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137325568"/>
+        <c:crossAx val="199530752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1089,7 +1092,7 @@
   <dimension ref="A2:V14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,7 +1341,9 @@
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="11"/>
-      <c r="U5" s="22"/>
+      <c r="U5" s="22" t="s">
+        <v>33</v>
+      </c>
       <c r="V5" s="23">
         <f>SUM(V3:V4)</f>
         <v>0.90285392507179341</v>

</xml_diff>

<commit_message>
Add PSD lessons learnt
</commit_message>
<xml_diff>
--- a/CS221/TimeLog.xlsx
+++ b/CS221/TimeLog.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="CS221" sheetId="1" r:id="rId1"/>
+    <sheet name="CS229" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -103,8 +103,42 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>jason chan</author>
+  </authors>
+  <commentList>
+    <comment ref="J8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>jason chan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+CB data export and prelim EDA</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Lectures</t>
   </si>
@@ -206,6 +240,12 @@
   </si>
   <si>
     <t>Overall</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Intro</t>
   </si>
 </sst>
 </file>
@@ -482,7 +522,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$2</c:f>
+              <c:f>'CS221'!$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -494,7 +534,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$3:$M$13</c:f>
+              <c:f>'CS221'!$M$3:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="11"/>
@@ -544,11 +584,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="199500544"/>
-        <c:axId val="199502080"/>
+        <c:axId val="137854976"/>
+        <c:axId val="137856512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="199500544"/>
+        <c:axId val="137854976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,7 +597,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199502080"/>
+        <c:crossAx val="137856512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -565,7 +605,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199502080"/>
+        <c:axId val="137856512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,7 +616,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199500544"/>
+        <c:crossAx val="137854976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -622,7 +662,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$2</c:f>
+              <c:f>'CS221'!$S$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -645,7 +685,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$3:$S$12</c:f>
+              <c:f>'CS221'!$S$3:$S$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -688,11 +728,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199530752"/>
-        <c:axId val="199536640"/>
+        <c:axId val="137876992"/>
+        <c:axId val="137878528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199530752"/>
+        <c:axId val="137876992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -701,7 +741,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199536640"/>
+        <c:crossAx val="137878528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -709,7 +749,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199536640"/>
+        <c:axId val="137878528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -720,7 +760,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199530752"/>
+        <c:crossAx val="137876992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1092,7 +1132,7 @@
   <dimension ref="A2:V14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1838,14 +1878,419 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="6">
+        <v>44733</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2" s="8">
+        <v>3</v>
+      </c>
+      <c r="G2" s="8">
+        <v>3</v>
+      </c>
+      <c r="H2" s="8">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8">
+        <v>0</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0</v>
+      </c>
+      <c r="K2" s="8">
+        <f>SUM(D2:J2)</f>
+        <v>6</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="19"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6">
+        <f>C2+7</f>
+        <v>44740</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8">
+        <v>0</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0</v>
+      </c>
+      <c r="K3" s="8">
+        <f t="shared" ref="K3:K8" si="0">SUM(D3:J3)</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="N3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="21"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6">
+        <f t="shared" ref="C4:C8" si="1">C3+7</f>
+        <v>44747</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0</v>
+      </c>
+      <c r="K4" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="N4" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="23"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6">
+        <f t="shared" si="1"/>
+        <v>44754</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0</v>
+      </c>
+      <c r="K5" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <f>A5+1</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6">
+        <f t="shared" si="1"/>
+        <v>44761</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <f t="shared" ref="A7:A8" si="2">A6+1</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6">
+        <f t="shared" si="1"/>
+        <v>44768</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0</v>
+      </c>
+      <c r="K7" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6">
+        <f t="shared" si="1"/>
+        <v>44775</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="K9" s="14">
+        <f>SUM(K2:K8)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>